<commit_message>
@21.02.22 Test case 4개 완료
</commit_message>
<xml_diff>
--- a/testData/LoginData.xlsx
+++ b/testData/LoginData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd9dc45417279bec/Project/seleniumFramework/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd9dc45417279bec/Project/Web_Test_Automation_Framework_V1/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04B51370-5CF2-4781-A2EB-62504588BCF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{04B51370-5CF2-4781-A2EB-62504588BCF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3D81811C-C3C6-4971-BF4F-920D4098D478}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="23040" windowHeight="12195" xr2:uid="{DBDEE73B-5FB7-4508-B237-803D4420C7BE}"/>
   </bookViews>
@@ -48,27 +48,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>admin@yourstore.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adm@yoursore.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Pass</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Fail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>centerho</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skyhigh1!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>centerhg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xyz</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -76,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +98,14 @@
       <color theme="10"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -131,7 +139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -452,7 +460,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -473,57 +481,51 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{836CC347-6093-4207-A7AC-6DBF5EA93ECF}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{6ABA351E-53FC-4DC4-87E3-31F8F4FF82FC}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{173FDB1B-DB4A-43CA-A9A8-030AE3CA0774}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{355A454D-CD0C-4F23-96E8-00D44B951188}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>